<commit_message>
Export btn working + borders in exported excel file closes #1
</commit_message>
<xml_diff>
--- a/SejtKemiRegning/SejtKemiRegning/bin/Debug/net5.0-windows/molMass.xlsx
+++ b/SejtKemiRegning/SejtKemiRegning/bin/Debug/net5.0-windows/molMass.xlsx
@@ -14,18 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <x:si>
-    <x:t>He</x:t>
+    <x:t>H3</x:t>
   </x:si>
   <x:si>
-    <x:t>H</x:t>
-  </x:si>
-  <x:si>
-    <x:t>N</x:t>
-  </x:si>
-  <x:si>
-    <x:t>O</x:t>
+    <x:t>Fe3</x:t>
   </x:si>
   <x:si>
     <x:t>Sum</x:t>
@@ -55,7 +49,7 @@
       <x:patternFill patternType="gray125"/>
     </x:fill>
   </x:fills>
-  <x:borders count="1">
+  <x:borders count="2">
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="none">
         <x:color rgb="FF000000"/>
@@ -67,6 +61,23 @@
         <x:color rgb="FF000000"/>
       </x:top>
       <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="thin">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="thin">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="thin">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="thin">
         <x:color rgb="FF000000"/>
       </x:bottom>
       <x:diagonal style="none">
@@ -74,13 +85,20 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -379,98 +397,34 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B11"/>
+  <x:dimension ref="A1:B4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:2">
-      <x:c r="A1" s="0" t="s">
+      <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="0" t="n">
-        <x:v>1</x:v>
+      <x:c r="B1" s="1" t="n">
+        <x:v>3.021</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2">
-      <x:c r="A2" s="0" t="s">
+      <x:c r="A2" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="n">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:2">
-      <x:c r="A3" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="n">
-        <x:v>3</x:v>
+      <x:c r="B2" s="1" t="n">
+        <x:v>167.535</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
-      <x:c r="A4" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="n">
+      <x:c r="A4" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
-    </x:row>
-    <x:row r="5" spans="1:2">
-      <x:c r="A5" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="n">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:2">
-      <x:c r="A6" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="n">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:2">
-      <x:c r="A7" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="n">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:2">
-      <x:c r="A8" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="n">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:2">
-      <x:c r="A9" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="n">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:2">
-      <x:c r="A10" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="n">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:2">
-      <x:c r="A11" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="n">
-        <x:v>38</x:v>
+      <x:c r="B4" s="1" t="n">
+        <x:v>170.556</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added exception handling for buttons
</commit_message>
<xml_diff>
--- a/SejtKemiRegning/SejtKemiRegning/bin/Debug/net5.0-windows/molMass.xlsx
+++ b/SejtKemiRegning/SejtKemiRegning/bin/Debug/net5.0-windows/molMass.xlsx
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <x:si>
     <x:t>H3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fe3</x:t>
   </x:si>
   <x:si>
     <x:t>Sum</x:t>
@@ -397,7 +394,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B4"/>
+  <x:dimension ref="A1:B3"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -411,20 +408,12 @@
         <x:v>3.021</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:2">
-      <x:c r="A2" s="1" t="s">
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B2" s="1" t="n">
-        <x:v>167.535</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:2">
-      <x:c r="A4" s="1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B4" s="1" t="n">
-        <x:v>170.556</x:v>
+      <x:c r="B3" s="1" t="n">
+        <x:v>3.021</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>